<commit_message>
hero skill icon fix
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HeroSkill.xlsx
+++ b/ConfigData/Xlsx/HeroSkill.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fish\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="HeroSkill" sheetId="1" r:id="rId1"/>
@@ -81,12 +81,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>chengjie</t>
-  </si>
-  <si>
-    <t>penhuo</t>
-  </si>
-  <si>
     <t>火箭</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -103,9 +97,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>dadun</t>
-  </si>
-  <si>
     <t>治疗</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -114,12 +105,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>zhiliao</t>
-  </si>
-  <si>
-    <t>miaozhun</t>
-  </si>
-  <si>
     <t>瞄准射击</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -136,9 +121,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>shibei</t>
-  </si>
-  <si>
     <t>探索</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -147,9 +129,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>yexing2</t>
-  </si>
-  <si>
     <t>背刺</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -158,7 +137,28 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>cisha</t>
+    <t>skill1</t>
+  </si>
+  <si>
+    <t>skill2</t>
+  </si>
+  <si>
+    <t>skill3</t>
+  </si>
+  <si>
+    <t>skill4</t>
+  </si>
+  <si>
+    <t>skill5</t>
+  </si>
+  <si>
+    <t>skill6</t>
+  </si>
+  <si>
+    <t>skill7</t>
+  </si>
+  <si>
+    <t>skill8</t>
   </si>
 </sst>
 </file>
@@ -833,74 +833,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -935,7 +867,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1217,17 +1149,17 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="12.25" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1247,7 +1179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1287,7 +1219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>31000001</v>
       </c>
@@ -1304,18 +1236,18 @@
         <v>52100000</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>31000002</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1324,18 +1256,18 @@
         <v>52100001</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>31000003</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1344,18 +1276,18 @@
         <v>53100005</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>31000004</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -1364,18 +1296,18 @@
         <v>53100002</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>31000005</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1387,15 +1319,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>31000006</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -1404,18 +1336,18 @@
         <v>53100000</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>31000007</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1424,18 +1356,18 @@
         <v>53100001</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>31000008</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -1444,7 +1376,7 @@
         <v>53100003</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remake the hero skill and relative card for defender
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HeroSkill.xlsx
+++ b/ConfigData/Xlsx/HeroSkill.xlsx
@@ -89,97 +89,97 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>治疗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复一个己方单位生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>瞄准射击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对一个单体目标造成魔法伤害，对英雄造成双倍伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>转化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗魔法值来获取一定的怒气值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>探索</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>一定概率抽一张牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>背刺</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对目标造成长时间的流血状态</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill1</t>
+  </si>
+  <si>
+    <t>skill2</t>
+  </si>
+  <si>
+    <t>skill3</t>
+  </si>
+  <si>
+    <t>skill4</t>
+  </si>
+  <si>
+    <t>skill5</t>
+  </si>
+  <si>
+    <t>skill6</t>
+  </si>
+  <si>
+    <t>skill7</t>
+  </si>
+  <si>
+    <t>skill8</t>
+  </si>
+  <si>
+    <t>skill9</t>
+  </si>
+  <si>
+    <t>亡灵</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在一个坟墓上召唤一个骷髅</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill10</t>
+  </si>
+  <si>
+    <t>图腾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在指定位置召唤一个图腾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>铁盾</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>可以给己方单位装备一面铁盾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>治疗</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>回复一个己方单位生命值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>瞄准射击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对一个单体目标造成魔法伤害，对英雄造成双倍伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>转化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>消耗魔法值来获取一定的怒气值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>探索</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>一定概率抽一张牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>背刺</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对目标造成长时间的流血状态</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill1</t>
-  </si>
-  <si>
-    <t>skill2</t>
-  </si>
-  <si>
-    <t>skill3</t>
-  </si>
-  <si>
-    <t>skill4</t>
-  </si>
-  <si>
-    <t>skill5</t>
-  </si>
-  <si>
-    <t>skill6</t>
-  </si>
-  <si>
-    <t>skill7</t>
-  </si>
-  <si>
-    <t>skill8</t>
-  </si>
-  <si>
-    <t>skill9</t>
-  </si>
-  <si>
-    <t>亡灵</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>在一个坟墓上召唤一个骷髅</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill10</t>
-  </si>
-  <si>
-    <t>图腾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>在指定位置召唤一个图腾</t>
+    <t>使我方王塔获得一些物甲</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1258,7 +1258,7 @@
         <v>52100000</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1266,19 +1266,19 @@
         <v>31000002</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>52100001</v>
+        <v>53100008</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1286,10 +1286,10 @@
         <v>31000003</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1298,7 +1298,7 @@
         <v>53100005</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1306,10 +1306,10 @@
         <v>31000004</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -1318,7 +1318,7 @@
         <v>53100002</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1326,10 +1326,10 @@
         <v>31000005</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1338,7 +1338,7 @@
         <v>53100004</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
         <v>53100000</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1366,10 +1366,10 @@
         <v>31000007</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1378,7 +1378,7 @@
         <v>53100001</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1386,10 +1386,10 @@
         <v>31000008</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -1398,7 +1398,7 @@
         <v>53100003</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1406,10 +1406,10 @@
         <v>31000009</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1418,7 +1418,7 @@
         <v>53100006</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1426,10 +1426,10 @@
         <v>31000010</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -1438,7 +1438,7 @@
         <v>53100007</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
balance the hero skill
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/HeroSkill.xlsx
+++ b/ConfigData/Xlsx/HeroSkill.xlsx
@@ -101,10 +101,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>对一个单体目标造成魔法伤害，对英雄造成双倍伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>转化</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -180,6 +176,10 @@
   </si>
   <si>
     <t>使我方王塔获得一些物甲</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对敌王塔造成魔法伤害</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1258,7 +1258,7 @@
         <v>52100000</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1266,10 +1266,10 @@
         <v>31000002</v>
       </c>
       <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
         <v>42</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1278,7 +1278,7 @@
         <v>53100008</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1286,10 +1286,10 @@
         <v>31000003</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1298,7 +1298,7 @@
         <v>53100005</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1309,7 +1309,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -1318,7 +1318,7 @@
         <v>53100002</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1326,10 +1326,10 @@
         <v>31000005</v>
       </c>
       <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1338,7 +1338,7 @@
         <v>53100004</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
         <v>53100000</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1378,7 +1378,7 @@
         <v>53100001</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1386,10 +1386,10 @@
         <v>31000008</v>
       </c>
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -1398,7 +1398,7 @@
         <v>53100003</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1406,10 +1406,10 @@
         <v>31000009</v>
       </c>
       <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1418,7 +1418,7 @@
         <v>53100006</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1426,10 +1426,10 @@
         <v>31000010</v>
       </c>
       <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
         <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -1438,7 +1438,7 @@
         <v>53100007</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>